<commit_message>
Adicionado os arquivos DDL, DML e DQL do exercício 1.1
</commit_message>
<xml_diff>
--- a/1.1-exercicio-pessoas/1.1-exercicio-pessoas.xlsx
+++ b/1.1-exercicio-pessoas/1.1-exercicio-pessoas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pichau\OneDrive\Desktop\exercicios-bd-sprint1\exercicios-sprint-1-bd\1.1-exercicio-pessoas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E26E0041-3EE5-4ACD-BDD7-84599C253D36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C055C9AA-7A4F-4FC3-91BC-C2791E7776B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9ED2761C-6859-4A3A-B345-4DFA045608C6}"/>
+    <workbookView xWindow="375" yWindow="2865" windowWidth="23970" windowHeight="11385" xr2:uid="{9ED2761C-6859-4A3A-B345-4DFA045608C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>Pessoa</t>
   </si>
@@ -569,23 +569,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66A0D024-73A8-4554-BE78-8965F0AEE38D}">
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" customWidth="1"/>
     <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -593,27 +595,15 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="J1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>9</v>
       </c>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
       <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="P1" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -629,47 +619,23 @@
       <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="7" t="s">
+      <c r="G2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="M2" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="N2" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="P2" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q2" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="R2" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="S2" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="15" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -685,49 +651,91 @@
       <c r="E3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="8">
+      <c r="G3" s="12">
         <v>1</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="H3" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="G7" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>1</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="8">
+      <c r="C9" s="8">
         <v>1</v>
       </c>
-      <c r="J3" s="12">
+      <c r="G9" s="16">
         <v>1</v>
       </c>
-      <c r="K3" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="M3" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="N3" s="12">
-        <v>1</v>
-      </c>
-      <c r="P3" s="16">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="17">
+      <c r="H9" s="17">
         <v>98938939</v>
       </c>
-      <c r="R3" s="17" t="s">
+      <c r="I9" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="S3" s="17" t="s">
+      <c r="J9" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="T3" s="16">
+      <c r="K9" s="16">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G3" r:id="rId1" xr:uid="{09C45B8E-F0A3-4091-890E-BA6B8B2DB612}"/>
+    <hyperlink ref="B9" r:id="rId1" xr:uid="{09C45B8E-F0A3-4091-890E-BA6B8B2DB612}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>